<commit_message>
vault backup: 2025-05-27 13:16:13
</commit_message>
<xml_diff>
--- a/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
+++ b/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc021263\Obsidian\NoahsObsidianSync\Chemistry\Year 12\Assignments\IA2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B42EA7AD-0B3E-4F0D-A2D1-8F7BFD0EC224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B56F8-09FE-4675-917C-A24A669087F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16020" activeTab="2" xr2:uid="{C5BF1A31-5F8B-4741-AA60-1E2AB135D676}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C5BF1A31-5F8B-4741-AA60-1E2AB135D676}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data IA2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2 (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2 (3)" sheetId="4" r:id="rId3"/>
+    <sheet name="Regular Processing" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
   <si>
     <t>Calculation prep</t>
   </si>
@@ -1458,7 +1458,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$2</c:f>
+              <c:f>'Sheet2 (3)'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1543,7 +1543,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$10</c:f>
+              <c:f>'Sheet2 (3)'!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1576,7 +1576,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$B$10</c:f>
+              <c:f>'Sheet2 (3)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1604,7 +1604,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D302-4E64-B637-44E4C99DA3CF}"/>
+              <c16:uniqueId val="{00000001-162C-411C-B3BB-9E244452639A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1613,7 +1613,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$1</c:f>
+              <c:f>'Sheet2 (3)'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1700,7 +1700,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$10</c:f>
+              <c:f>'Sheet2 (3)'!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1733,7 +1733,628 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$E$3:$E$10</c:f>
+              <c:f>'Sheet2 (3)'!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.68066666666666664</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49466666666666664</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48133333333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.44133333333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-162C-411C-B3BB-9E244452639A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="515641471"/>
+        <c:axId val="515641951"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="515641471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515641951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="515641951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515641471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average vs trial 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.7152411398412872E-2"/>
+          <c:y val="0.1670646058947497"/>
+          <c:w val="0.74009022253418799"/>
+          <c:h val="0.72880370672233563"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Regular Processing'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10383625770388795"/>
+                  <c:y val="-5.4526293753538582E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Regular Processing'!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Regular Processing'!$B$3:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.70299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D302-4E64-B637-44E4C99DA3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Regular Processing'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.8318115497489521E-2"/>
+                  <c:y val="0.18812701141964996"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Regular Processing'!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Regular Processing'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2109,6 +2730,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3142,6 +3803,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3742,6 +4919,49 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>539994</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>326570</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>18143</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13B2A678-5CDE-4DA4-AE3E-50C8CAE53A3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4441,10 +5661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DDC99A-BD69-4F85-A6ED-057A7D0863C9}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScale="77" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="138" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4699,7 +5919,7 @@
         <v>0.4306666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.4</v>
       </c>
@@ -4708,7 +5928,7 @@
         <v>0.42199999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.3</v>
       </c>
@@ -4717,7 +5937,7 @@
         <v>0.48133333333333334</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.2</v>
       </c>
@@ -4726,12 +5946,76 @@
         <v>0.44800000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.1</v>
       </c>
       <c r="B20">
         <f t="shared" si="2"/>
+        <v>0.44133333333333336</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.68066666666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0.85</v>
+      </c>
+      <c r="E24">
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0.7</v>
+      </c>
+      <c r="E25">
+        <v>0.49466666666666664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E26">
+        <v>0.4306666666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0.4</v>
+      </c>
+      <c r="E27">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0.3</v>
+      </c>
+      <c r="E28">
+        <v>0.48133333333333334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>0.2</v>
+      </c>
+      <c r="E29">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+      <c r="E30">
         <v>0.44133333333333336</v>
       </c>
     </row>
@@ -4743,11 +6027,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D75EC8-0243-465F-A593-A949321AC039}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E36CC3E-7FF4-4ABC-8A3B-BC88E1C19814}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="223" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScale="141" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5037,4 +6321,301 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D75EC8-0243-465F-A593-A949321AC039}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView zoomScale="134" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="D3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>0.68066666666666664</v>
+      </c>
+      <c r="F3">
+        <f>(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
+        <v>2.0999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.85</v>
+      </c>
+      <c r="B4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.623</v>
+      </c>
+      <c r="D4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="0">AVERAGE(B4:D4)</f>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="1">(MAX(B4:D4)-MIN(B4:D4))*0.5</f>
+        <v>8.8000000000000023E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.7</v>
+      </c>
+      <c r="B5">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.49466666666666664</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C6">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.41749999999999998</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.500000000000004E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="C7">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8">
+        <v>0.498</v>
+      </c>
+      <c r="C8">
+        <v>0.47</v>
+      </c>
+      <c r="D8">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.48133333333333334</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999984E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.44133333333333336</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f>E3</f>
+        <v>0.68066666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.85</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B20" si="2">E4</f>
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.7</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>0.49466666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>0.41749999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.4</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.3</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>0.48133333333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.1</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>0.44133333333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-05-28 05:24:58
</commit_message>
<xml_diff>
--- a/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
+++ b/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data IA2" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Sheet2 (2)" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Sheet2 (3)" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="OutliersRemoved" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Regular Processing" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t xml:space="preserve">Calculation prep</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">Average voltage (V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trial number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage</t>
   </si>
 </sst>
 </file>
@@ -480,11 +486,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="66066170"/>
-        <c:axId val="85415390"/>
+        <c:axId val="64424357"/>
+        <c:axId val="60358368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66066170"/>
+        <c:axId val="64424357"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -570,12 +576,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85415390"/>
+        <c:crossAx val="60358368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85415390"/>
+        <c:axId val="60358368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +667,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66066170"/>
+        <c:crossAx val="64424357"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1051,11 +1057,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2432863"/>
-        <c:axId val="7942334"/>
+        <c:axId val="39335513"/>
+        <c:axId val="47304025"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2432863"/>
+        <c:axId val="39335513"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,12 +1104,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7942334"/>
+        <c:crossAx val="47304025"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7942334"/>
+        <c:axId val="47304025"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1152,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2432863"/>
+        <c:crossAx val="39335513"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1258,7 +1264,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet2 (3)'!$B$2</c:f>
+              <c:f>OutliersRemoved!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1341,7 +1347,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet2 (3)'!$A$3:$A$10</c:f>
+              <c:f>OutliersRemoved!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1374,7 +1380,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet2 (3)'!$B$3:$B$10</c:f>
+              <c:f>OutliersRemoved!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1386,6 +1392,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.557</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.457</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.438</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.498</c:v>
@@ -1406,7 +1418,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet2 (3)'!$E$1</c:f>
+              <c:f>OutliersRemoved!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1489,7 +1501,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet2 (3)'!$A$3:$A$10</c:f>
+              <c:f>OutliersRemoved!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1522,7 +1534,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet2 (3)'!$E$3:$E$10</c:f>
+              <c:f>OutliersRemoved!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1536,16 +1548,16 @@
                   <c:v>0.494666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4175</c:v>
+                  <c:v>0.430666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.414</c:v>
+                  <c:v>0.422</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.481333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.448</c:v>
+                  <c:v>0.4725</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.441333333333333</c:v>
@@ -1555,11 +1567,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="11923860"/>
-        <c:axId val="65458753"/>
+        <c:axId val="31068497"/>
+        <c:axId val="66313363"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11923860"/>
+        <c:axId val="31068497"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,12 +1614,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65458753"/>
+        <c:crossAx val="66313363"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65458753"/>
+        <c:axId val="66313363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1662,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11923860"/>
+        <c:crossAx val="31068497"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2059,11 +2071,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20618511"/>
-        <c:axId val="60699800"/>
+        <c:axId val="75817315"/>
+        <c:axId val="952588"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20618511"/>
+        <c:axId val="75817315"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2106,12 +2118,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60699800"/>
+        <c:crossAx val="952588"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60699800"/>
+        <c:axId val="952588"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2166,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20618511"/>
+        <c:crossAx val="75817315"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2526,8 +2538,8 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="E21:G23 I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="1" sqref="E18:F40 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2877,8 +2889,8 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21:G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="E18:F40 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3242,10 +3254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="1" sqref="E21:G23 G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="E18:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3350,6 +3362,9 @@
       <c r="A6" s="1" t="n">
         <v>0.55</v>
       </c>
+      <c r="B6" s="1" t="n">
+        <v>0.457</v>
+      </c>
       <c r="C6" s="1" t="n">
         <v>0.422</v>
       </c>
@@ -3358,17 +3373,20 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">AVERAGE(B6:D6)</f>
-        <v>0.4175</v>
+        <v>0.430666666666667</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">(MAX(B6:D6)-MIN(B6:D6))*0.5</f>
-        <v>0.0045</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>0.4</v>
       </c>
+      <c r="B7" s="1" t="n">
+        <v>0.438</v>
+      </c>
       <c r="C7" s="1" t="n">
         <v>0.412</v>
       </c>
@@ -3377,11 +3395,11 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">AVERAGE(B7:D7)</f>
-        <v>0.414</v>
+        <v>0.422</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">(MAX(B7:D7)-MIN(B7:D7))*0.5</f>
-        <v>0.002</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,16 +3434,14 @@
       <c r="C9" s="1" t="n">
         <v>0.487</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>0.399</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="n">
         <f aca="false">AVERAGE(B9:D9)</f>
-        <v>0.448</v>
+        <v>0.4725</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">(MAX(B9:D9)-MIN(B9:D9))*0.5</f>
-        <v>0.044</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,7 +3507,7 @@
       </c>
       <c r="B16" s="1" t="n">
         <f aca="false">E6</f>
-        <v>0.4175</v>
+        <v>0.430666666666667</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,7 +3516,13 @@
       </c>
       <c r="B17" s="1" t="n">
         <f aca="false">E7</f>
-        <v>0.414</v>
+        <v>0.422</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3511,6 +3533,12 @@
         <f aca="false">E8</f>
         <v>0.481333333333333</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>0.703</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -3518,7 +3546,13 @@
       </c>
       <c r="B19" s="1" t="n">
         <f aca="false">E9</f>
-        <v>0.448</v>
+        <v>0.4725</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0.664</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3528,6 +3562,172 @@
       <c r="B20" s="1" t="n">
         <f aca="false">E10</f>
         <v>0.441333333333333</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>0.557</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>0.457</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0.458</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>0.405</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>0.678</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>0.455</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>0.422</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0.412</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0.487</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0.456</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>0.661</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>0.488</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>0.472</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>0.413</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>0.416</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>0.476</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>0.463</v>
       </c>
     </row>
   </sheetData>
@@ -3549,8 +3749,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="1" sqref="E21:G23 G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="1" sqref="E18:F40 G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
vault backup: 2025-06-03 14:01:05
</commit_message>
<xml_diff>
--- a/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
+++ b/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
@@ -1,20 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc021263\Obsidian\NoahsObsidianSync\Chemistry\Year 12\Assignments\IA2\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A5F7F3-D9E0-413B-A6EE-1496E3B06846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Raw data IA2" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2 (2)" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="OutliersRemoved" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Regular Processing" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Raw data IA2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="OutliersRemoved" sheetId="3" r:id="rId3"/>
+    <sheet name="Regular Processing" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,110 +41,68 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
-    <t xml:space="preserve">Calculation prep</t>
+    <t>Calculation prep</t>
   </si>
   <si>
-    <t xml:space="preserve">Voltage</t>
+    <t>Voltage</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean</t>
+    <t>Mean</t>
   </si>
   <si>
-    <t xml:space="preserve">absolute error</t>
+    <t>absolute error</t>
   </si>
   <si>
-    <t xml:space="preserve">Mols</t>
+    <t>Mols</t>
   </si>
   <si>
-    <t xml:space="preserve">Amount of CuSO4 (ml)</t>
+    <t>Amount of CuSO4 (ml)</t>
   </si>
   <si>
-    <t xml:space="preserve">H2O amount (ml)</t>
+    <t>H2O amount (ml)</t>
   </si>
   <si>
-    <t xml:space="preserve">Trail 1</t>
+    <t>Trail 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Trial 2</t>
+    <t>Trial 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Trial 3</t>
+    <t>Trial 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Absolute error (%)</t>
+    <t>Absolute error (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">sigma</t>
+    <t>sigma</t>
   </si>
   <si>
-    <t xml:space="preserve">Trial 1</t>
+    <t>Trial 1</t>
   </si>
   <si>
     <t xml:space="preserve">Mols </t>
   </si>
   <si>
-    <t xml:space="preserve">Average voltage (V)</t>
+    <t>Average voltage (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">trial number</t>
+    <t>trial number</t>
   </si>
   <si>
-    <t xml:space="preserve">voltage</t>
+    <t>voltage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +114,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -148,57 +122,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -257,15 +197,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -274,30 +232,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+              <a:defRPr sz="1300" b="0" u="none" strike="noStrike">
                 <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" strike="noStrike" u="none">
+              <a:rPr lang="en-US" sz="1400" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:uFillTx/>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
-              <a:t>Concentration</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" strike="noStrike" u="none">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:t> vs Voltage Produced</a:t>
+              <a:t>Concentration vs Voltage Produced</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -312,6 +260,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -330,9 +279,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -347,12 +293,19 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -360,6 +313,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -368,26 +322,27 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
                   <a:srgbClr val="156082"/>
                 </a:solidFill>
@@ -396,14 +351,15 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="log"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
                   <a:srgbClr val="156082"/>
                 </a:solidFill>
@@ -413,10 +369,11 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -434,7 +391,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -458,34 +415,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.680666666666667</c:v>
+                  <c:v>0.68066666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.591666666666667</c:v>
+                  <c:v>0.59166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.494666666666667</c:v>
+                  <c:v>0.49466666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.430666666666667</c:v>
+                  <c:v>0.4306666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.422</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.481333333333333</c:v>
+                  <c:v>0.48133333333333334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.448</c:v>
+                  <c:v>0.44800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.441333333333333</c:v>
+                  <c:v>0.44133333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8044-4468-ABC7-3077123AE5E9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="91911850"/>
         <c:axId val="22995199"/>
       </c:scatterChart>
@@ -500,7 +470,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -513,30 +483,20 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                  <a:defRPr sz="1300" b="0" u="none" strike="noStrike">
                     <a:uFillTx/>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-GB" sz="1000" strike="noStrike" u="none">
+                  <a:rPr lang="en-GB" sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:rPr>
-                  <a:t>Concentration</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr b="0" lang="en-GB" sz="1000" strike="noStrike" u="none">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Aptos Narrow"/>
-                  </a:rPr>
-                  <a:t> of CuSO4</a:t>
+                  <a:t>Concentration of CuSO4</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -556,7 +516,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -566,7 +526,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -574,6 +534,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="22995199"/>
@@ -591,7 +552,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -604,30 +565,20 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+                  <a:defRPr sz="1300" b="0" u="none" strike="noStrike">
                     <a:uFillTx/>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" lang="en-GB" sz="1000" strike="noStrike" u="none">
+                  <a:rPr lang="en-GB" sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
                     <a:uFillTx/>
                     <a:latin typeface="Aptos Narrow"/>
                   </a:rPr>
-                  <a:t>Cell</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr b="0" lang="en-GB" sz="1000" strike="noStrike" u="none">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:uFillTx/>
-                    <a:latin typeface="Aptos Narrow"/>
-                  </a:rPr>
-                  <a:t> Potential (ECell) (V)</a:t>
+                  <a:t>Cell Potential (ECell) (V)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -647,7 +598,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -657,7 +608,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -665,6 +616,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="91911850"/>
@@ -680,25 +632,33 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -707,13 +667,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+              <a:defRPr sz="1300" b="0" u="none" strike="noStrike">
                 <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" strike="noStrike" u="none">
+              <a:rPr lang="en-US" sz="1400" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -740,10 +700,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.057155451072583"/>
-          <c:y val="0.167033773861968"/>
+          <c:x val="5.7155451072582998E-2"/>
+          <c:y val="0.16703377386196799"/>
           <c:w val="0.740033303947497"/>
-          <c:h val="0.72870778267254"/>
+          <c:h val="0.72870778267253999"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -764,9 +724,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -781,12 +738,19 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -794,6 +758,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -802,26 +767,27 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
                   <a:srgbClr val="156082"/>
                 </a:solidFill>
@@ -830,10 +796,11 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -851,7 +818,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -875,16 +842,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.703</c:v>
+                  <c:v>0.70299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.664</c:v>
+                  <c:v>0.66400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.557</c:v>
+                  <c:v>0.55700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.457</c:v>
+                  <c:v>0.45700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.438</c:v>
@@ -893,15 +860,20 @@
                   <c:v>0.498</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.458</c:v>
+                  <c:v>0.45800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.405</c:v>
+                  <c:v>0.40500000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-190B-4EA0-BC2F-B6F076D686F1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -918,9 +890,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="e97132"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -930,17 +899,24 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="e97132"/>
+                <a:srgbClr val="E97132"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -948,6 +924,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -956,38 +933,40 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
-                  <a:srgbClr val="e97132"/>
+                  <a:srgbClr val="E97132"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
                 <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1005,7 +984,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -1029,34 +1008,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.680666666666667</c:v>
+                  <c:v>0.68066666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.591666666666667</c:v>
+                  <c:v>0.59166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.494666666666667</c:v>
+                  <c:v>0.49466666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.430666666666667</c:v>
+                  <c:v>0.4306666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.422</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.481333333333333</c:v>
+                  <c:v>0.48133333333333334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.448</c:v>
+                  <c:v>0.44800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.441333333333333</c:v>
+                  <c:v>0.44133333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-190B-4EA0-BC2F-B6F076D686F1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="2700541"/>
         <c:axId val="31682550"/>
       </c:scatterChart>
@@ -1071,7 +1063,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1084,7 +1076,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1094,7 +1086,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1102,6 +1094,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="31682550"/>
@@ -1119,7 +1112,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1132,7 +1125,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1142,7 +1135,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1150,6 +1143,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2700541"/>
@@ -1177,7 +1171,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+            <a:defRPr sz="900" b="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -1185,30 +1179,39 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1217,13 +1220,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+              <a:defRPr sz="1300" b="0" u="none" strike="noStrike">
                 <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" strike="noStrike" u="none">
+              <a:rPr lang="en-US" sz="1400" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1250,10 +1253,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.057155451072583"/>
-          <c:y val="0.167033773861968"/>
+          <c:x val="5.7155451072582998E-2"/>
+          <c:y val="0.16703377386196799"/>
           <c:w val="0.740033303947497"/>
-          <c:h val="0.72870778267254"/>
+          <c:h val="0.72870778267253999"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1274,9 +1277,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -1291,12 +1291,19 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1304,6 +1311,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1312,26 +1320,27 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
                   <a:srgbClr val="156082"/>
                 </a:solidFill>
@@ -1340,10 +1349,11 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1361,7 +1371,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -1385,16 +1395,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.703</c:v>
+                  <c:v>0.70299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.664</c:v>
+                  <c:v>0.66400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.557</c:v>
+                  <c:v>0.55700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.457</c:v>
+                  <c:v>0.45700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.438</c:v>
@@ -1403,15 +1413,20 @@
                   <c:v>0.498</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.458</c:v>
+                  <c:v>0.45800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.405</c:v>
+                  <c:v>0.40500000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-95CD-4607-8FBD-47CC019B5383}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1428,9 +1443,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="e97132"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -1440,17 +1452,24 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="e97132"/>
+                <a:srgbClr val="E97132"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1458,6 +1477,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1466,38 +1486,40 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
-                  <a:srgbClr val="e97132"/>
+                  <a:srgbClr val="E97132"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
                 <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1515,7 +1537,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -1539,34 +1561,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.680666666666667</c:v>
+                  <c:v>0.68066666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.591666666666667</c:v>
+                  <c:v>0.59166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.494666666666667</c:v>
+                  <c:v>0.49466666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.430666666666667</c:v>
+                  <c:v>0.4306666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.422</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.481333333333333</c:v>
+                  <c:v>0.48133333333333334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4725</c:v>
+                  <c:v>0.47250000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.441333333333333</c:v>
+                  <c:v>0.44133333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-95CD-4607-8FBD-47CC019B5383}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="23232619"/>
         <c:axId val="28117379"/>
       </c:scatterChart>
@@ -1581,7 +1616,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1594,7 +1629,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1604,7 +1639,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1612,6 +1647,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="28117379"/>
@@ -1629,7 +1665,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1642,7 +1678,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1652,7 +1688,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1660,6 +1696,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="23232619"/>
@@ -1687,7 +1724,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+            <a:defRPr sz="900" b="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -1695,30 +1732,39 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1727,13 +1773,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" strike="noStrike" u="none">
+              <a:defRPr sz="1300" b="0" u="none" strike="noStrike">
                 <a:uFillTx/>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" strike="noStrike" u="none">
+              <a:rPr lang="en-US" sz="1400" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1760,10 +1806,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.057155451072583"/>
-          <c:y val="0.167033773861968"/>
+          <c:x val="5.7155451072582998E-2"/>
+          <c:y val="0.16703377386196799"/>
           <c:w val="0.740033303947497"/>
-          <c:h val="0.72870778267254"/>
+          <c:h val="0.72870778267253999"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1784,9 +1830,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="156082"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -1801,12 +1844,19 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1814,6 +1864,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1822,26 +1873,27 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
                   <a:srgbClr val="156082"/>
                 </a:solidFill>
@@ -1850,10 +1902,11 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1871,7 +1924,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -1895,27 +1948,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.703</c:v>
+                  <c:v>0.70299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.664</c:v>
+                  <c:v>0.66400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.557</c:v>
+                  <c:v>0.55700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.498</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.458</c:v>
+                  <c:v>0.45800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.405</c:v>
+                  <c:v>0.40500000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3FC9-4B53-91D9-3D1772023F5C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1932,9 +1990,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="e97132"/>
-            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -1944,17 +1999,24 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="e97132"/>
+                <a:srgbClr val="E97132"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                  <a:defRPr sz="1000" b="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -1962,6 +2024,7 @@
                     <a:latin typeface="Aptos Narrow"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1970,38 +2033,40 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="25560">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="25560">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                    </a:ln>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
-                  <a:srgbClr val="e97132"/>
+                  <a:srgbClr val="E97132"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
                 <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -2019,7 +2084,7 @@
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -2043,34 +2108,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.680666666666667</c:v>
+                  <c:v>0.68066666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.591666666666667</c:v>
+                  <c:v>0.59166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.494666666666667</c:v>
+                  <c:v>0.49466666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4175</c:v>
+                  <c:v>0.41749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.414</c:v>
+                  <c:v>0.41399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.481333333333333</c:v>
+                  <c:v>0.48133333333333334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.448</c:v>
+                  <c:v>0.44800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.441333333333333</c:v>
+                  <c:v>0.44133333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3FC9-4B53-91D9-3D1772023F5C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="12063174"/>
         <c:axId val="68066242"/>
       </c:scatterChart>
@@ -2085,7 +2163,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2098,7 +2176,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2108,7 +2186,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2116,6 +2194,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="68066242"/>
@@ -2133,7 +2212,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2146,7 +2225,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="BFBFBF"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2156,7 +2235,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+              <a:defRPr sz="900" b="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2164,6 +2243,7 @@
                 <a:latin typeface="Aptos Narrow"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="12063174"/>
@@ -2191,7 +2271,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" strike="noStrike" u="none">
+            <a:defRPr sz="900" b="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -2199,28 +2279,35 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2234,14 +2321,20 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1381680" y="2175480"/>
-        <a:ext cx="5235120" cy="2877840"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2255,7 +2348,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -2269,14 +2362,20 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8033040" y="504360"/>
-        <a:ext cx="7350120" cy="2941560"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2290,7 +2389,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -2304,14 +2403,20 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8033040" y="504360"/>
-        <a:ext cx="7350120" cy="2941560"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2325,7 +2430,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -2339,14 +2444,20 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8033040" y="504360"/>
-        <a:ext cx="7350120" cy="2941560"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2360,54 +2471,54 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -2439,7 +2550,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -2463,7 +2574,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2523,346 +2634,345 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.14"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3">
         <v>50</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>0.703</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.678</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0.661</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <f aca="false">AVERAGE(D3:F3)</f>
-        <v>0.680666666666667</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <f aca="false">(MAX(D3:F3)-MIN(D3:F3))/2</f>
-        <v>0.021</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <f aca="false">H3*100</f>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="D3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="E3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="F3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G10" si="0">AVERAGE(D3:F3)</f>
+        <v>0.68066666666666664</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="1">(MAX(D3:F3)-MIN(D3:F3))/2</f>
+        <v>2.0999999999999963E-2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="2">H3*100</f>
+        <v>2.0999999999999961</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>0.85</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <f aca="false">A4*50/1</f>
+      <c r="B4">
+        <f t="shared" ref="B4:B10" si="3">A4*50/1</f>
         <v>42.5</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <f aca="false">50-B4</f>
+      <c r="C4">
+        <f t="shared" ref="C4:C10" si="4">50-B4</f>
         <v>7.5</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>0.664</v>
-      </c>
-      <c r="E4" s="1" t="n">
+      <c r="D4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="E4">
         <v>0.623</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <f aca="false">AVERAGE(D4:F4)</f>
-        <v>0.591666666666667</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <f aca="false">(MAX(D4:F4)-MIN(D4:F4))/2</f>
-        <v>0.088</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <f aca="false">H4*100</f>
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="F4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000023E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>8.8000000000000025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>0.7</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <f aca="false">A5*50/1</f>
+      <c r="B5">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <f aca="false">50-B5</f>
+      <c r="C5">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>0.557</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.455</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.472</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <f aca="false">AVERAGE(D5:F5)</f>
-        <v>0.494666666666667</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <f aca="false">(MAX(D5:F5)-MIN(D5:F5))/2</f>
-        <v>0.051</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <f aca="false">H5*100</f>
-        <v>5.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <f aca="false">A6*50/1</f>
-        <v>27.5</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <f aca="false">50-B6</f>
-        <v>22.5</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.413</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <f aca="false">AVERAGE(D6:F6)</f>
-        <v>0.430666666666667</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <f aca="false">(MAX(D6:F6)-MIN(D6:F6))/2</f>
-        <v>0.022</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <f aca="false">H6*100</f>
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="D5">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="E5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="F5">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.49466666666666664</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000018E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>5.1000000000000014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="3"/>
+        <v>27.500000000000004</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="4"/>
+        <v>22.499999999999996</v>
+      </c>
+      <c r="D6">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="E6">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.4306666666666667</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2.200000000000002E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>2.200000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>0.4</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <f aca="false">A7*50/1</f>
+      <c r="B7">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <f aca="false">50-B7</f>
+      <c r="C7">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7">
         <v>0.438</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.416</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <f aca="false">AVERAGE(D7:F7)</f>
-        <v>0.422</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <f aca="false">(MAX(D7:F7)-MIN(D7:F7))/2</f>
-        <v>0.013</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <f aca="false">H7*100</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="E7">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1.3000000000000012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>0.3</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <f aca="false">A8*50/1</f>
+      <c r="B8">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <f aca="false">50-B8</f>
+      <c r="C8">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8">
         <v>0.498</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8">
         <v>0.47</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>0.476</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <f aca="false">AVERAGE(D8:F8)</f>
-        <v>0.481333333333333</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <f aca="false">(MAX(D8:F8)-MIN(D8:F8))/2</f>
-        <v>0.014</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <f aca="false">H8*100</f>
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="F8">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.48133333333333334</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1.4000000000000012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>0.2</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <f aca="false">A9*50/1</f>
+      <c r="B9">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <f aca="false">50-B9</f>
+      <c r="C9">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>0.458</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>0.399</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <f aca="false">AVERAGE(D9:F9)</f>
-        <v>0.448</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <f aca="false">(MAX(D9:F9)-MIN(D9:F9))/2</f>
-        <v>0.044</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <f aca="false">H9*100</f>
-        <v>4.4</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="D9">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="E9">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999984E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>0.1</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <f aca="false">A10*50/1</f>
+      <c r="B10">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <f aca="false">50-B10</f>
+      <c r="C10">
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="D10" s="1" t="n">
-        <v>0.405</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>0.456</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <f aca="false">AVERAGE(D10:F10)</f>
-        <v>0.441333333333333</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <f aca="false">(MAX(D10:F10)-MIN(D10:F10))/2</f>
-        <v>0.029</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <f aca="false">H10*100</f>
+      <c r="D10">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="E10">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.44133333333333336</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
         <v>2.9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="n">
-        <f aca="false">B3+B4+B5+B6+B7+B8+B9+B10</f>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>B3+B4+B5+B6+B7+B8+B9+B10</f>
         <v>205</v>
       </c>
     </row>
@@ -2871,1178 +2981,1172 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>0.703</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.678</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.661</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">AVERAGE(B3:D3)</f>
-        <v>0.680666666666667</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <f aca="false">(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
-        <v>0.021</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="B3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="D3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">AVERAGE(B3:D3)</f>
+        <v>0.68066666666666664</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
+        <v>2.0999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>0.85</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>0.664</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="B4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="C4">
         <v>0.623</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">AVERAGE(B4:D4)</f>
-        <v>0.591666666666667</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">(MAX(B4:D4)-MIN(B4:D4))*0.5</f>
-        <v>0.088</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="D4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000023E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>0.7</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0.557</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0.455</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0.472</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <f aca="false">AVERAGE(B5:D5)</f>
-        <v>0.494666666666667</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">(MAX(B5:D5)-MIN(B5:D5))*0.5</f>
-        <v>0.051</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.413</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <f aca="false">AVERAGE(B6:D6)</f>
-        <v>0.430666666666667</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <f aca="false">(MAX(B6:D6)-MIN(B6:D6))*0.5</f>
-        <v>0.022</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="B5">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.49466666666666664</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B6">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.4306666666666667</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2.200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>0.4</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7">
         <v>0.438</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.416</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <f aca="false">AVERAGE(B7:D7)</f>
-        <v>0.422</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <f aca="false">(MAX(B7:D7)-MIN(B7:D7))*0.5</f>
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="C7">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>0.3</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8">
         <v>0.498</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8">
         <v>0.47</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>0.476</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <f aca="false">AVERAGE(B8:D8)</f>
+      <c r="D8">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.48133333333333334</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999984E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.44133333333333336</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.68066666666666698</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.85</v>
+      </c>
+      <c r="B14">
+        <v>0.59166666666666701</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.7</v>
+      </c>
+      <c r="B15">
+        <v>0.49466666666666698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B16">
+        <v>0.43066666666666698</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.4</v>
+      </c>
+      <c r="B17">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.3</v>
+      </c>
+      <c r="B18">
         <v>0.481333333333333</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">(MAX(B8:D8)-MIN(B8:D8))*0.5</f>
-        <v>0.014</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>0.2</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>0.458</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.399</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <f aca="false">AVERAGE(B9:D9)</f>
-        <v>0.448</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <f aca="false">(MAX(B9:D9)-MIN(B9:D9))*0.5</f>
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="B19">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>0.1</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>0.405</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>0.456</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <f aca="false">AVERAGE(B10:D10)</f>
-        <v>0.441333333333333</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <f aca="false">(MAX(B10:D10)-MIN(B10:D10))*0.5</f>
-        <v>0.029</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="B20">
+        <v>0.44133333333333302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>0.680666666666667</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="E23">
+        <v>0.68066666666666698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24">
         <v>0.85</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <v>0.591666666666667</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="E24">
+        <v>0.59166666666666701</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25">
         <v>0.7</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <v>0.494666666666667</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>0.430666666666667</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="E25">
+        <v>0.49466666666666698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E26">
+        <v>0.43066666666666698</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27">
         <v>0.4</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>0.422</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="E27">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28">
         <v>0.3</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="E28">
         <v>0.481333333333333</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29">
         <v>0.2</v>
       </c>
-      <c r="B19" s="1" t="n">
-        <v>0.448</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="E29">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30">
         <v>0.1</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <v>0.441333333333333</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>0.680666666666667</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>0.591666666666667</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>0.494666666666667</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>0.430666666666667</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>0.422</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>0.481333333333333</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>0.448</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>0.441333333333333</v>
+      <c r="E30">
+        <v>0.44133333333333302</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>0.703</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.678</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.661</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">AVERAGE(B3:D3)</f>
-        <v>0.680666666666667</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <f aca="false">(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
-        <v>0.021</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="B3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="D3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">AVERAGE(B3:D3)</f>
+        <v>0.68066666666666664</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
+        <v>2.0999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>0.85</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>0.664</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="B4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="C4">
         <v>0.623</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">AVERAGE(B4:D4)</f>
-        <v>0.591666666666667</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">(MAX(B4:D4)-MIN(B4:D4))*0.5</f>
-        <v>0.088</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="D4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000023E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>0.7</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0.557</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0.455</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0.472</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <f aca="false">AVERAGE(B5:D5)</f>
-        <v>0.494666666666667</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">(MAX(B5:D5)-MIN(B5:D5))*0.5</f>
-        <v>0.051</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.413</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <f aca="false">AVERAGE(B6:D6)</f>
-        <v>0.430666666666667</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <f aca="false">(MAX(B6:D6)-MIN(B6:D6))*0.5</f>
-        <v>0.022</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="B5">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.49466666666666664</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B6">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.4306666666666667</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2.200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>0.4</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7">
         <v>0.438</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.416</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <f aca="false">AVERAGE(B7:D7)</f>
-        <v>0.422</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <f aca="false">(MAX(B7:D7)-MIN(B7:D7))*0.5</f>
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="C7">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>0.3</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8">
         <v>0.498</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8">
         <v>0.47</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>0.476</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <f aca="false">AVERAGE(B8:D8)</f>
-        <v>0.481333333333333</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">(MAX(B8:D8)-MIN(B8:D8))*0.5</f>
-        <v>0.014</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="D8">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.48133333333333334</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>0.2</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>0.458</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="n">
-        <f aca="false">AVERAGE(B9:D9)</f>
-        <v>0.4725</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <f aca="false">(MAX(B9:D9)-MIN(B9:D9))*0.5</f>
-        <v>0.0145</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="B9">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.47250000000000003</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.4499999999999985E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>0.1</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>0.405</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>0.456</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <f aca="false">AVERAGE(B10:D10)</f>
-        <v>0.441333333333333</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <f aca="false">(MAX(B10:D10)-MIN(B10:D10))*0.5</f>
-        <v>0.029</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="B10">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.44133333333333336</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <f aca="false">E3</f>
-        <v>0.680666666666667</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="B13">
+        <f t="shared" ref="B13:B20" si="2">E3</f>
+        <v>0.68066666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>0.85</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <f aca="false">E4</f>
-        <v>0.591666666666667</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>0.7</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <f aca="false">E5</f>
-        <v>0.494666666666667</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <f aca="false">E6</f>
-        <v>0.430666666666667</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>0.49466666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>0.4306666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>0.4</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <f aca="false">E7</f>
-        <v>0.422</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E17" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>0.3</v>
       </c>
-      <c r="B18" s="1" t="n">
-        <f aca="false">E8</f>
-        <v>0.481333333333333</v>
-      </c>
-      <c r="E18" s="1" t="n">
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>0.48133333333333334</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="1" t="n">
-        <v>0.703</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="F18">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>0.2</v>
       </c>
-      <c r="B19" s="1" t="n">
-        <f aca="false">E9</f>
-        <v>0.4725</v>
-      </c>
-      <c r="E19" s="1" t="n">
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>0.47250000000000003</v>
+      </c>
+      <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="1" t="n">
-        <v>0.664</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="F19">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>0.1</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <f aca="false">E10</f>
-        <v>0.441333333333333</v>
-      </c>
-      <c r="E20" s="1" t="n">
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>0.44133333333333336</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="1" t="n">
-        <v>0.557</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E21" s="1" t="n">
+      <c r="F20">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I20">
+        <f>AVERAGE(F18:F25)</f>
+        <v>0.52250000000000008</v>
+      </c>
+      <c r="J20">
+        <f>(MAX(F18:F25)-MIN(F18:F25))*0.5</f>
+        <v>0.14899999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <v>0.457</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E22" s="1" t="n">
+      <c r="F21">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="I21">
+        <f>AVERAGE(F26:F33)</f>
+        <v>0.50037500000000013</v>
+      </c>
+      <c r="J21">
+        <f>(MAX(F26:F33)-MIN(F26:F33))*0.5</f>
+        <v>0.13300000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22">
         <v>0.438</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E23" s="1" t="n">
+      <c r="I22">
+        <f>AVERAGE(F34:F41)</f>
+        <v>0.4841428571428571</v>
+      </c>
+      <c r="J22">
+        <f>(MAX(F34:F41)-MIN(F34:F41))*0.5</f>
+        <v>0.12400000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23">
         <v>0.498</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E24" s="1" t="n">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>0.458</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E25" s="1" t="n">
+      <c r="F24">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="1" t="n">
-        <v>0.405</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E26" s="1" t="n">
+      <c r="F25">
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26">
         <v>2</v>
       </c>
-      <c r="F26" s="1" t="n">
-        <v>0.678</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E27" s="1" t="n">
+      <c r="F26">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27">
         <v>2</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27">
         <v>0.623</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E28" s="1" t="n">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28">
         <v>2</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <v>0.455</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E29" s="1" t="n">
+      <c r="F28">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29">
         <v>2</v>
       </c>
-      <c r="F29" s="1" t="n">
-        <v>0.422</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E30" s="1" t="n">
+      <c r="F29">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30">
         <v>2</v>
       </c>
-      <c r="F30" s="1" t="n">
-        <v>0.412</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E31" s="1" t="n">
+      <c r="F30">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31">
         <v>2</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31">
         <v>0.47</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E32" s="1" t="n">
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32">
         <v>2</v>
       </c>
-      <c r="F32" s="1" t="n">
-        <v>0.487</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E33" s="1" t="n">
+      <c r="F32">
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33">
         <v>2</v>
       </c>
-      <c r="F33" s="1" t="n">
-        <v>0.456</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="1" t="n">
+      <c r="F33">
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34">
         <v>3</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>0.661</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E35" s="1" t="n">
+      <c r="F34">
+        <v>0.66100000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35">
         <v>3</v>
       </c>
-      <c r="F35" s="1" t="n">
-        <v>0.488</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E36" s="1" t="n">
+      <c r="F35">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36">
         <v>3</v>
       </c>
-      <c r="F36" s="1" t="n">
-        <v>0.472</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E37" s="1" t="n">
+      <c r="F36">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37">
         <v>3</v>
       </c>
-      <c r="F37" s="1" t="n">
-        <v>0.413</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E38" s="1" t="n">
+      <c r="F37">
+        <v>0.41299999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38">
         <v>3</v>
       </c>
-      <c r="F38" s="1" t="n">
-        <v>0.416</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E39" s="1" t="n">
+      <c r="F38">
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39">
         <v>3</v>
       </c>
-      <c r="F39" s="1" t="n">
-        <v>0.476</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E40" s="1" t="n">
+      <c r="F39">
+        <v>0.47599999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40">
         <v>3</v>
       </c>
-      <c r="F40" s="1" t="n">
-        <v>0.463</v>
+      <c r="F40">
+        <v>0.46300000000000002</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>0.703</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.678</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.661</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">AVERAGE(B3:D3)</f>
-        <v>0.680666666666667</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <f aca="false">(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
-        <v>0.021</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="B3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="D3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">AVERAGE(B3:D3)</f>
+        <v>0.68066666666666664</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">(MAX(B3:D3)-MIN(B3:D3))*0.5</f>
+        <v>2.0999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>0.85</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>0.664</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="B4">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="C4">
         <v>0.623</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">AVERAGE(B4:D4)</f>
-        <v>0.591666666666667</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">(MAX(B4:D4)-MIN(B4:D4))*0.5</f>
-        <v>0.088</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="D4">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000023E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>0.7</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0.557</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0.455</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0.472</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <f aca="false">AVERAGE(B5:D5)</f>
-        <v>0.494666666666667</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">(MAX(B5:D5)-MIN(B5:D5))*0.5</f>
-        <v>0.051</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0.422</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.413</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <f aca="false">AVERAGE(B6:D6)</f>
-        <v>0.4175</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <f aca="false">(MAX(B6:D6)-MIN(B6:D6))*0.5</f>
-        <v>0.0045</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="B5">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D5">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.49466666666666664</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.1000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C6">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.41749999999999998</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.500000000000004E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>0.4</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.416</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <f aca="false">AVERAGE(B7:D7)</f>
-        <v>0.414</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <f aca="false">(MAX(B7:D7)-MIN(B7:D7))*0.5</f>
-        <v>0.002</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="C7">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>0.3</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8">
         <v>0.498</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8">
         <v>0.47</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>0.476</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <f aca="false">AVERAGE(B8:D8)</f>
-        <v>0.481333333333333</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">(MAX(B8:D8)-MIN(B8:D8))*0.5</f>
-        <v>0.014</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="D8">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.48133333333333334</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>0.2</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>0.458</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.399</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <f aca="false">AVERAGE(B9:D9)</f>
-        <v>0.448</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <f aca="false">(MAX(B9:D9)-MIN(B9:D9))*0.5</f>
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="B9">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999984E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>0.1</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>0.405</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>0.456</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <f aca="false">AVERAGE(B10:D10)</f>
-        <v>0.441333333333333</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <f aca="false">(MAX(B10:D10)-MIN(B10:D10))*0.5</f>
-        <v>0.029</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="B10">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.44133333333333336</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <f aca="false">E3</f>
-        <v>0.680666666666667</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="B13">
+        <f t="shared" ref="B13:B20" si="2">E3</f>
+        <v>0.68066666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>0.85</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <f aca="false">E4</f>
-        <v>0.591666666666667</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>0.7</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <f aca="false">E5</f>
-        <v>0.494666666666667</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <f aca="false">E6</f>
-        <v>0.4175</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>0.49466666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>0.41749999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>0.4</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <f aca="false">E7</f>
-        <v>0.414</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>0.3</v>
       </c>
-      <c r="B18" s="1" t="n">
-        <f aca="false">E8</f>
-        <v>0.481333333333333</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>0.48133333333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>0.2</v>
       </c>
-      <c r="B19" s="1" t="n">
-        <f aca="false">E9</f>
-        <v>0.448</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>0.1</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <f aca="false">E10</f>
-        <v>0.441333333333333</v>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>0.44133333333333336</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-06-03 14:01:50
</commit_message>
<xml_diff>
--- a/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
+++ b/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc021263\Obsidian\NoahsObsidianSync\Chemistry\Year 12\Assignments\IA2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A5F7F3-D9E0-413B-A6EE-1496E3B06846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE523B5-76DD-4EF9-A601-5A2AC496D1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1764,6 +1764,467 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.43192084938924774"/>
+                  <c:y val="-0.12969578243834984"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>OutliersRemoved!$J$20:$J$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.14899999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.13300000000000003</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12400000000000003</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>OutliersRemoved!$J$20:$J$22</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.14899999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.13300000000000003</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12400000000000003</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OutliersRemoved!$H$20:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OutliersRemoved!$I$20:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.52250000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50037500000000013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4841428571428571</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5500-4CD4-BF1A-CF0ABBC50AE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="826214031"/>
+        <c:axId val="826213071"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="826214031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="826213071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="826213071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="826214031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
     <c:title>
@@ -2306,6 +2767,562 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2421,6 +3438,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>270711</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>92242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>270711</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>168442</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25BB0F8F-7342-F2B1-65D5-0F41229D71F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3348,10 +4401,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="G15" zoomScale="185" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3662,6 +4715,9 @@
       <c r="F20">
         <v>0.55700000000000005</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
       <c r="I20">
         <f>AVERAGE(F18:F25)</f>
         <v>0.52250000000000008</v>
@@ -3678,6 +4734,9 @@
       <c r="F21">
         <v>0.45700000000000002</v>
       </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
       <c r="I21">
         <f>AVERAGE(F26:F33)</f>
         <v>0.50037500000000013</v>
@@ -3694,6 +4753,9 @@
       <c r="F22">
         <v>0.438</v>
       </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
       <c r="I22">
         <f>AVERAGE(F34:F41)</f>
         <v>0.4841428571428571</v>
@@ -3783,7 +4845,7 @@
         <v>0.48699999999999999</v>
       </c>
     </row>
-    <row r="33" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>2</v>
       </c>
@@ -3791,7 +4853,7 @@
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="34" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>3</v>
       </c>
@@ -3799,7 +4861,7 @@
         <v>0.66100000000000003</v>
       </c>
     </row>
-    <row r="35" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>3</v>
       </c>
@@ -3807,7 +4869,7 @@
         <v>0.48799999999999999</v>
       </c>
     </row>
-    <row r="36" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>3</v>
       </c>
@@ -3815,7 +4877,7 @@
         <v>0.47199999999999998</v>
       </c>
     </row>
-    <row r="37" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>3</v>
       </c>
@@ -3823,7 +4885,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="38" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>3</v>
       </c>
@@ -3831,15 +4893,18 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="39" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>3</v>
       </c>
       <c r="F39">
         <v>0.47599999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>0.99219999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
vault backup: 2025-06-04 07:09:31
</commit_message>
<xml_diff>
--- a/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
+++ b/Chemistry/Year 12/Assignments/IA2/Results/Chemistry experiment data IA2 (version 1).xlsx
@@ -92,13 +92,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,6 +136,18 @@
       <sz val="10"/>
       <color rgb="FF595959"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFE6E905"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -208,10 +219,10 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFE6E905"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -258,7 +269,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -481,11 +492,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="8222932"/>
-        <c:axId val="2594547"/>
+        <c:axId val="28523546"/>
+        <c:axId val="26728342"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8222932"/>
+        <c:axId val="28523546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,12 +572,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2594547"/>
+        <c:crossAx val="26728342"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2594547"/>
+        <c:axId val="26728342"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -642,7 +653,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8222932"/>
+        <c:crossAx val="28523546"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -717,7 +728,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.0571737315192298"/>
           <c:y val="0.167054216130217"/>
-          <c:w val="0.740016700230856"/>
+          <c:w val="0.739967581904809"/>
           <c:h val="0.728674580834659"/>
         </c:manualLayout>
       </c:layout>
@@ -1032,11 +1043,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16698165"/>
-        <c:axId val="82283437"/>
+        <c:axId val="30416271"/>
+        <c:axId val="4712988"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16698165"/>
+        <c:axId val="30416271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,12 +1090,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82283437"/>
+        <c:crossAx val="4712988"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82283437"/>
+        <c:axId val="4712988"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,7 +1138,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16698165"/>
+        <c:crossAx val="30416271"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1227,7 +1238,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.0571737315192298"/>
           <c:y val="0.167054216130217"/>
-          <c:w val="0.740016700230856"/>
+          <c:w val="0.739967581904809"/>
           <c:h val="0.728674580834659"/>
         </c:manualLayout>
       </c:layout>
@@ -1542,11 +1553,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52271108"/>
-        <c:axId val="94614552"/>
+        <c:axId val="3938031"/>
+        <c:axId val="76993271"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52271108"/>
+        <c:axId val="3938031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,12 +1600,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94614552"/>
+        <c:crossAx val="76993271"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94614552"/>
+        <c:axId val="76993271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1637,7 +1648,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52271108"/>
+        <c:crossAx val="3938031"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1820,56 +1831,6 @@
             <c:dispEq val="1"/>
           </c:trendline>
           <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>OutliersRemoved!$J$20:$J$22</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>0.149</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.133</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.124</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>OutliersRemoved!$J$20:$J$22</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>0.149</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.133</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.124</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
@@ -1941,11 +1902,7 @@
               <a:srgbClr val="ff420e"/>
             </a:solidFill>
             <a:ln w="12600">
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1957,7 +1914,41 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="ff420e"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" strike="noStrike" u="none">
+                      <a:uFillTx/>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
             <c:txPr>
               <a:bodyPr wrap="none"/>
               <a:lstStyle/>
@@ -1970,6 +1961,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1992,6 +1984,20 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="ff420e"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>OutliersRemoved!$H$20:$H$22</c:f>
@@ -2046,11 +2052,7 @@
               <a:srgbClr val="ffd320"/>
             </a:solidFill>
             <a:ln w="10080">
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -2097,6 +2099,18 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>OutliersRemoved!$H$20:$H$22</c:f>
@@ -2132,11 +2146,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86576026"/>
-        <c:axId val="81547953"/>
+        <c:axId val="40534737"/>
+        <c:axId val="75318291"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86576026"/>
+        <c:axId val="40534737"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,12 +2193,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81547953"/>
+        <c:crossAx val="75318291"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81547953"/>
+        <c:axId val="75318291"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,14 +2241,16 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86576026"/>
+        <c:crossAx val="40534737"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln w="0">
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
@@ -2327,7 +2343,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.0571737315192298"/>
           <c:y val="0.167054216130217"/>
-          <c:w val="0.740016700230856"/>
+          <c:w val="0.739967581904809"/>
           <c:h val="0.728674580834659"/>
         </c:manualLayout>
       </c:layout>
@@ -2636,11 +2652,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="93369849"/>
-        <c:axId val="5316011"/>
+        <c:axId val="20893436"/>
+        <c:axId val="26946310"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93369849"/>
+        <c:axId val="20893436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2683,12 +2699,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5316011"/>
+        <c:crossAx val="26946310"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5316011"/>
+        <c:axId val="26946310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2731,7 +2747,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93369849"/>
+        <c:crossAx val="20893436"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2797,7 +2813,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>493200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>99720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2805,7 +2821,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1379880" y="2175480"/>
+        <a:off x="1379880" y="2007720"/>
         <a:ext cx="5228280" cy="2877480"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2831,8 +2847,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>325080</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2840,7 +2856,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8015400" y="504360"/>
+        <a:off x="8015400" y="474120"/>
         <a:ext cx="7328880" cy="2941200"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2866,8 +2882,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>340920</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2889,15 +2905,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>552600</xdr:colOff>
+      <xdr:colOff>563040</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>552240</xdr:colOff>
+      <xdr:colOff>562680</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2905,7 +2921,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7342200" y="5106960"/>
+        <a:off x="7352640" y="4814280"/>
         <a:ext cx="5486040" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2931,8 +2947,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>325080</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2940,7 +2956,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8015400" y="504360"/>
+        <a:off x="8015400" y="474120"/>
         <a:ext cx="7328880" cy="2941200"/>
       </xdr:xfrm>
       <a:graphic>
@@ -2997,14 +3013,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -3012,67 +3028,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -3091,35 +3065,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -3133,7 +3083,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -3144,7 +3094,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +3112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3185,7 +3135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -3217,7 +3167,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -3251,7 +3201,7 @@
         <v>8.8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -3285,7 +3235,7 @@
         <v>5.1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -3319,7 +3269,7 @@
         <v>2.2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -3353,7 +3303,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -3387,7 +3337,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -3421,7 +3371,7 @@
         <v>4.4</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -3455,7 +3405,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <f aca="false">B3+B4+B5+B6+B7+B8+B9+B10</f>
         <v>205</v>
@@ -3484,7 +3434,7 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -3493,7 +3443,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>4</v>
       </c>
@@ -3509,7 +3459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
@@ -3520,7 +3470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -3542,7 +3492,7 @@
         <v>0.021</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -3564,7 +3514,7 @@
         <v>0.088</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -3586,7 +3536,7 @@
         <v>0.051</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -3608,7 +3558,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -3630,7 +3580,7 @@
         <v>0.013</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -3652,7 +3602,7 @@
         <v>0.014</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -3674,7 +3624,7 @@
         <v>0.044</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -3696,7 +3646,7 @@
         <v>0.029</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
@@ -3704,7 +3654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1</v>
       </c>
@@ -3712,7 +3662,7 @@
         <v>0.680666666666667</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -3720,7 +3670,7 @@
         <v>0.591666666666667</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -3728,7 +3678,7 @@
         <v>0.494666666666667</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -3736,7 +3686,7 @@
         <v>0.430666666666667</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -3744,7 +3694,7 @@
         <v>0.422</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -3752,7 +3702,7 @@
         <v>0.481333333333333</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -3760,7 +3710,7 @@
         <v>0.448</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -3768,7 +3718,7 @@
         <v>0.441333333333333</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="n">
         <v>1</v>
       </c>
@@ -3776,7 +3726,7 @@
         <v>0.680666666666667</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -3784,7 +3734,7 @@
         <v>0.591666666666667</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -3792,7 +3742,7 @@
         <v>0.494666666666667</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -3800,7 +3750,7 @@
         <v>0.430666666666667</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -3808,7 +3758,7 @@
         <v>0.422</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -3816,7 +3766,7 @@
         <v>0.481333333333333</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -3824,7 +3774,7 @@
         <v>0.448</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -3851,8 +3801,8 @@
   </sheetPr>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D14" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3860,7 +3810,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>4</v>
       </c>
@@ -3876,7 +3826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
@@ -3887,7 +3837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -3909,7 +3859,7 @@
         <v>0.021</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -3931,7 +3881,7 @@
         <v>0.088</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -3953,7 +3903,7 @@
         <v>0.051</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -3975,7 +3925,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -3997,7 +3947,7 @@
         <v>0.013</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -4019,7 +3969,7 @@
         <v>0.014</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -4038,7 +3988,7 @@
         <v>0.0145</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -4060,7 +4010,7 @@
         <v>0.029</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
@@ -4068,7 +4018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1</v>
       </c>
@@ -4077,7 +4027,7 @@
         <v>0.680666666666667</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -4086,7 +4036,7 @@
         <v>0.591666666666667</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -4095,7 +4045,7 @@
         <v>0.494666666666667</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -4104,7 +4054,7 @@
         <v>0.430666666666667</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -4119,7 +4069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -4134,7 +4084,7 @@
         <v>0.703</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -4161,7 +4111,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -4404,7 +4354,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -4413,7 +4363,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>4</v>
       </c>
@@ -4429,7 +4379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
@@ -4440,7 +4390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
@@ -4462,7 +4412,7 @@
         <v>0.021</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -4484,7 +4434,7 @@
         <v>0.088</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -4506,7 +4456,7 @@
         <v>0.051</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -4525,7 +4475,7 @@
         <v>0.0045</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -4544,7 +4494,7 @@
         <v>0.002</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -4566,7 +4516,7 @@
         <v>0.014</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -4588,7 +4538,7 @@
         <v>0.044</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -4610,7 +4560,7 @@
         <v>0.029</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
@@ -4618,7 +4568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1</v>
       </c>
@@ -4627,7 +4577,7 @@
         <v>0.680666666666667</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0.85</v>
       </c>
@@ -4636,7 +4586,7 @@
         <v>0.591666666666667</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -4645,7 +4595,7 @@
         <v>0.494666666666667</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>0.55</v>
       </c>
@@ -4654,7 +4604,7 @@
         <v>0.4175</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>0.4</v>
       </c>
@@ -4663,7 +4613,7 @@
         <v>0.414</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>0.3</v>
       </c>
@@ -4672,7 +4622,7 @@
         <v>0.481333333333333</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>0.2</v>
       </c>
@@ -4681,7 +4631,7 @@
         <v>0.448</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>0.1</v>
       </c>

</xml_diff>